<commit_message>
[UPDATE]: Updating leaderboard data
</commit_message>
<xml_diff>
--- a/public/assets/data/leaderboard.xlsx
+++ b/public/assets/data/leaderboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhijit\Desktop\GenAI2k24\public\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E480578-6D6F-4FDE-9A53-3B675983D4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2145B5D3-66AB-41C7-87E0-30D004F3D5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F7EEA724-8D90-4E29-9D32-49F4243CC7C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{258733F0-FC3F-4135-AC78-BFFC1EC78B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Indian Institute of Engineering" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="569">
   <si>
     <t>User Name</t>
   </si>
@@ -295,6 +295,9 @@
     <t>https://www.cloudskillsboost.google/public_profiles/12627f23-75c7-4ac9-84a2-13fb86e486b5</t>
   </si>
   <si>
+    <t>Diwali in The Arcade [Game]</t>
+  </si>
+  <si>
     <t>Harsh Prasad</t>
   </si>
   <si>
@@ -313,198 +316,201 @@
     <t>https://www.cloudskillsboost.google/public_profiles/ba2fa9f4-be0c-4a14-88fd-a85f8dd1bde0</t>
   </si>
   <si>
+    <t>Wadadare Piyush Rajendra</t>
+  </si>
+  <si>
+    <t>wadadarepiyush@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/d7f5622a-1532-416a-952f-2132ce32cc3a</t>
+  </si>
+  <si>
+    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge]</t>
+  </si>
+  <si>
+    <t>shaileshkumarj2004@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/538e38d4-73c2-4cd0-9710-dfd783386748</t>
+  </si>
+  <si>
+    <t>Harsh Kumar Sah</t>
+  </si>
+  <si>
+    <t>sahharsh787@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/4815e3c5-5cb8-499d-92be-455f448252a3</t>
+  </si>
+  <si>
+    <t>sarthak23062003@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/df60ec1d-69de-427f-82d5-651ae75322b5</t>
+  </si>
+  <si>
+    <t>Ankit Kumar</t>
+  </si>
+  <si>
+    <t>anki95kr@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/5bef10aa-518b-48d2-b506-e02d1b520d12</t>
+  </si>
+  <si>
+    <t>Divyansh Srivastav</t>
+  </si>
+  <si>
+    <t>srivastavmohit9876@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/84bba77a-b11b-4fe5-b56e-8f7c60f5be7f</t>
+  </si>
+  <si>
+    <t>Ankit kumar</t>
+  </si>
+  <si>
+    <t>ankitmishra0917@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/7cbdc2e4-060a-4114-bdd6-33cae60f2ed7</t>
+  </si>
+  <si>
+    <t>Ayush Dutta</t>
+  </si>
+  <si>
+    <t>ayushiiestsgdsc@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/b8a5831f-ffbe-42d4-aaaa-b1ada5b20261</t>
+  </si>
+  <si>
+    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with Pub/Sub [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Get Started with Google Workspace Tools [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge] | App Engine: 3 Ways [Skill Badge] | Cloud Speech API: 3 Ways [Skill Badge] | Monitoring in Google Cloud [Skill Badge] | Networking Fundamentals on Google Cloud [Skill Badge] | Analyze Images with the Cloud Vision API [Skill Badge] | Prompt Design in Vertex AI [Skill Badge] | Develop GenAI Apps with Gemini and Streamlit [Skill Badge]</t>
+  </si>
+  <si>
+    <t>Mehul Mehta</t>
+  </si>
+  <si>
+    <t>mehulmehta17113346@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/f3a03eea-56c9-4c79-8bdd-235bf7845f2c</t>
+  </si>
+  <si>
+    <t>Yasharth Shukla</t>
+  </si>
+  <si>
+    <t>yasharthshukla01@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/ed886629-dd50-40ee-bb40-b6c1f65e55ca</t>
+  </si>
+  <si>
+    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Get Started with Google Workspace Tools [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge] | App Engine: 3 Ways [Skill Badge] | Cloud Speech API: 3 Ways [Skill Badge]</t>
+  </si>
+  <si>
+    <t>Devojeet Vyapari</t>
+  </si>
+  <si>
+    <t>2024meb069.devojeet@students.iiests.ac.in</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/b91d8349-cc06-4d77-b972-d7b65a64fb9c</t>
+  </si>
+  <si>
+    <t>Ashika Shaw</t>
+  </si>
+  <si>
+    <t>ashikashaw1505@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/37489f87-bf04-4275-822d-8e9d717f77f8</t>
+  </si>
+  <si>
+    <t>Rupak Jana</t>
+  </si>
+  <si>
+    <t>studyrupakh@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/6f115d34-bccc-4e6a-9e2e-8f52bad7f4c9</t>
+  </si>
+  <si>
+    <t>Arham Owais</t>
+  </si>
+  <si>
+    <t>arham2004.owais@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/40f80402-d840-464d-b082-f821c841c2ae</t>
+  </si>
+  <si>
+    <t>SANTOSH</t>
+  </si>
+  <si>
+    <t>santosh.csb084.mail@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/c3569fd0-b38c-433a-ae29-ee2a0b7a155d</t>
+  </si>
+  <si>
+    <t>Vipin Kumar Chaudhary</t>
+  </si>
+  <si>
+    <t>vipinjietb070@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/6bef4b12-e47b-444f-8d07-6b6156220332</t>
+  </si>
+  <si>
+    <t>Tapash Jaiswal</t>
+  </si>
+  <si>
+    <t>2023csb046.tapash@students.iiests.ac.in</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/a1fae5ef-1abe-4cc2-bd0e-08b58b4bd757</t>
+  </si>
+  <si>
+    <t>Soureen karmakar</t>
+  </si>
+  <si>
+    <t>2023itb075.soureen@students.iiests.ac.in</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/6ec301b6-6525-4b13-9129-767e3e3a5a13</t>
+  </si>
+  <si>
+    <t>Ankur Mukherjee</t>
+  </si>
+  <si>
+    <t>mukherjeeankur0073@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/6de2f67f-45c2-4f89-9230-ac8a4e3ae631</t>
+  </si>
+  <si>
+    <t>Vaibhav Singh</t>
+  </si>
+  <si>
+    <t>vaibhavdmcsingh@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/e7594041-90e9-41fc-9e18-a874c20a39fe</t>
+  </si>
+  <si>
+    <t>Subhoshri Pal</t>
+  </si>
+  <si>
+    <t>cordeliaherondale720@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/c4075567-e71b-4582-a195-a3f01034b09d</t>
+  </si>
+  <si>
     <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge]</t>
   </si>
   <si>
-    <t>Wadadare Piyush Rajendra</t>
-  </si>
-  <si>
-    <t>wadadarepiyush@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/d7f5622a-1532-416a-952f-2132ce32cc3a</t>
-  </si>
-  <si>
-    <t>shaileshkumarj2004@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/538e38d4-73c2-4cd0-9710-dfd783386748</t>
-  </si>
-  <si>
-    <t>Harsh Kumar Sah</t>
-  </si>
-  <si>
-    <t>sahharsh787@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/4815e3c5-5cb8-499d-92be-455f448252a3</t>
-  </si>
-  <si>
-    <t>sarthak23062003@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/df60ec1d-69de-427f-82d5-651ae75322b5</t>
-  </si>
-  <si>
-    <t>Ankit Kumar</t>
-  </si>
-  <si>
-    <t>anki95kr@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/5bef10aa-518b-48d2-b506-e02d1b520d12</t>
-  </si>
-  <si>
-    <t>Divyansh Srivastav</t>
-  </si>
-  <si>
-    <t>srivastavmohit9876@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/84bba77a-b11b-4fe5-b56e-8f7c60f5be7f</t>
-  </si>
-  <si>
-    <t>Ankit kumar</t>
-  </si>
-  <si>
-    <t>ankitmishra0917@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/7cbdc2e4-060a-4114-bdd6-33cae60f2ed7</t>
-  </si>
-  <si>
-    <t>Ayush Dutta</t>
-  </si>
-  <si>
-    <t>ayushiiestsgdsc@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/b8a5831f-ffbe-42d4-aaaa-b1ada5b20261</t>
-  </si>
-  <si>
-    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with Pub/Sub [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Get Started with Google Workspace Tools [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge] | App Engine: 3 Ways [Skill Badge] | Cloud Speech API: 3 Ways [Skill Badge] | Monitoring in Google Cloud [Skill Badge] | Networking Fundamentals on Google Cloud [Skill Badge] | Analyze Images with the Cloud Vision API [Skill Badge] | Prompt Design in Vertex AI [Skill Badge] | Develop GenAI Apps with Gemini and Streamlit [Skill Badge]</t>
-  </si>
-  <si>
-    <t>Mehul Mehta</t>
-  </si>
-  <si>
-    <t>mehulmehta17113346@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/f3a03eea-56c9-4c79-8bdd-235bf7845f2c</t>
-  </si>
-  <si>
-    <t>Yasharth Shukla</t>
-  </si>
-  <si>
-    <t>yasharthshukla01@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/ed886629-dd50-40ee-bb40-b6c1f65e55ca</t>
-  </si>
-  <si>
-    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Get Started with Google Workspace Tools [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge]</t>
-  </si>
-  <si>
-    <t>Devojeet Vyapari</t>
-  </si>
-  <si>
-    <t>2024meb069.devojeet@students.iiests.ac.in</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/b91d8349-cc06-4d77-b972-d7b65a64fb9c</t>
-  </si>
-  <si>
-    <t>Ashika Shaw</t>
-  </si>
-  <si>
-    <t>ashikashaw1505@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/37489f87-bf04-4275-822d-8e9d717f77f8</t>
-  </si>
-  <si>
-    <t>Rupak Jana</t>
-  </si>
-  <si>
-    <t>studyrupakh@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/6f115d34-bccc-4e6a-9e2e-8f52bad7f4c9</t>
-  </si>
-  <si>
-    <t>Arham Owais</t>
-  </si>
-  <si>
-    <t>arham2004.owais@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/40f80402-d840-464d-b082-f821c841c2ae</t>
-  </si>
-  <si>
-    <t>SANTOSH</t>
-  </si>
-  <si>
-    <t>santosh.csb084.mail@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/c3569fd0-b38c-433a-ae29-ee2a0b7a155d</t>
-  </si>
-  <si>
-    <t>Vipin Kumar Chaudhary</t>
-  </si>
-  <si>
-    <t>vipinjietb070@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/6bef4b12-e47b-444f-8d07-6b6156220332</t>
-  </si>
-  <si>
-    <t>Tapash Jaiswal</t>
-  </si>
-  <si>
-    <t>2023csb046.tapash@students.iiests.ac.in</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/a1fae5ef-1abe-4cc2-bd0e-08b58b4bd757</t>
-  </si>
-  <si>
-    <t>Soureen karmakar</t>
-  </si>
-  <si>
-    <t>2023itb075.soureen@students.iiests.ac.in</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/6ec301b6-6525-4b13-9129-767e3e3a5a13</t>
-  </si>
-  <si>
-    <t>Ankur Mukherjee</t>
-  </si>
-  <si>
-    <t>mukherjeeankur0073@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/6de2f67f-45c2-4f89-9230-ac8a4e3ae631</t>
-  </si>
-  <si>
-    <t>Vaibhav Singh</t>
-  </si>
-  <si>
-    <t>vaibhavdmcsingh@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/e7594041-90e9-41fc-9e18-a874c20a39fe</t>
-  </si>
-  <si>
-    <t>Subhoshri Pal</t>
-  </si>
-  <si>
-    <t>cordeliaherondale720@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/c4075567-e71b-4582-a195-a3f01034b09d</t>
-  </si>
-  <si>
     <t>Tejas Pawar</t>
   </si>
   <si>
@@ -808,6 +814,9 @@
     <t>https://www.cloudskillsboost.google/public_profiles/c4e8b98b-826e-495a-a234-3ce32f33c997</t>
   </si>
   <si>
+    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with Pub/Sub [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge]</t>
+  </si>
+  <si>
     <t>Subhrajyoti Sarkar</t>
   </si>
   <si>
@@ -1051,9 +1060,6 @@
     <t>https://www.cloudskillsboost.google/public_profiles/a073b57c-88d3-4699-8f85-7c6266f84ee0</t>
   </si>
   <si>
-    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge]</t>
-  </si>
-  <si>
     <t>Mohit Yadav</t>
   </si>
   <si>
@@ -1465,16 +1471,13 @@
     <t>https://www.cloudskillsboost.google/public_profiles/ef2329d4-0d26-49f5-b3c6-301f7f0b86be</t>
   </si>
   <si>
-    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge] | App Engine: 3 Ways [Skill Badge] | Cloud Speech API: 3 Ways [Skill Badge] | Monitoring in Google Cloud [Skill Badge]</t>
+    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Dataplex [Skill Badge] | Get Started with Google Workspace Tools [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge] | App Engine: 3 Ways [Skill Badge] | Cloud Speech API: 3 Ways [Skill Badge] | Monitoring in Google Cloud [Skill Badge] | Networking Fundamentals on Google Cloud [Skill Badge]</t>
   </si>
   <si>
     <t>a.kumarishalu113@gmail.com</t>
   </si>
   <si>
     <t>https://www.cloudskillsboost.google/public_profiles/7bcc7efb-3170-4f57-8789-4c0441853705</t>
-  </si>
-  <si>
-    <t>The Basics of Google Cloud Compute [Skill Badge] | Get Started with Cloud Storage [Skill Badge] | Get Started with Pub/Sub [Skill Badge] | Get Started with API Gateway [Skill Badge] | Get Started with Looker [Skill Badge] | Get Started with Google Workspace Tools [Skill Badge] | Cloud Functions: 3 Ways [Skill Badge] | App Engine: 3 Ways [Skill Badge] | Cloud Speech API: 3 Ways [Skill Badge] | Monitoring in Google Cloud [Skill Badge] | Analyze Images with the Cloud Vision API [Skill Badge] | Prompt Design in Vertex AI [Skill Badge] | Develop GenAI Apps with Gemini and Streamlit [Skill Badge]</t>
   </si>
   <si>
     <t>Liya Mufizraza Shabbir</t>
@@ -2563,7 +2566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F89BA-4D58-436E-B576-B398CE3596AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BC980D-5199-4875-BF2C-E548BEABAC29}">
   <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3250,18 +3253,21 @@
         <v>25</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -3276,7 +3282,7 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -3290,10 +3296,10 @@
         <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -3305,10 +3311,10 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H27" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -3331,16 +3337,16 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -3351,10 +3357,10 @@
         <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -3374,13 +3380,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -3403,10 +3409,10 @@
         <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -3429,13 +3435,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -3455,13 +3461,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -3481,13 +3487,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
         <v>13</v>
@@ -3507,13 +3513,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -3528,7 +3534,7 @@
         <v>15</v>
       </c>
       <c r="H35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -3539,13 +3545,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
@@ -3565,13 +3571,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -3583,10 +3589,10 @@
         <v>15</v>
       </c>
       <c r="G37">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3594,13 +3600,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
@@ -3620,13 +3626,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -3646,13 +3652,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -3672,13 +3678,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -3698,13 +3704,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
@@ -3724,13 +3730,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D43" t="s">
         <v>13</v>
@@ -3750,13 +3756,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C44" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -3771,7 +3777,7 @@
         <v>15</v>
       </c>
       <c r="H44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -3782,13 +3788,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -3811,13 +3817,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -3840,13 +3846,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D47" t="s">
         <v>13</v>
@@ -3861,7 +3867,7 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -3872,13 +3878,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
         <v>13</v>
@@ -3893,7 +3899,7 @@
         <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -3904,13 +3910,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
@@ -3930,13 +3936,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C50" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
@@ -3956,13 +3962,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B51" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C51" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
         <v>13</v>
@@ -3985,13 +3991,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
         <v>13</v>
@@ -4011,13 +4017,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B53" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C53" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -4032,7 +4038,7 @@
         <v>8</v>
       </c>
       <c r="H53" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -4040,13 +4046,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C54" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D54" t="s">
         <v>13</v>
@@ -4066,13 +4072,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B55" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C55" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D55" t="s">
         <v>13</v>
@@ -4092,13 +4098,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B56" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C56" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -4118,13 +4124,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D57" t="s">
         <v>13</v>
@@ -4150,13 +4156,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B58" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C58" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -4176,13 +4182,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B59" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C59" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -4205,13 +4211,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D60" t="s">
         <v>13</v>
@@ -4226,7 +4232,7 @@
         <v>5</v>
       </c>
       <c r="H60" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -4237,13 +4243,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -4258,7 +4264,7 @@
         <v>9</v>
       </c>
       <c r="H61" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -4269,13 +4275,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B62" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -4295,13 +4301,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B63" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C63" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -4316,7 +4322,7 @@
         <v>7</v>
       </c>
       <c r="H63" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -4324,13 +4330,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B64" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C64" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -4342,7 +4348,10 @@
         <v>15</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>60</v>
       </c>
       <c r="I64">
         <v>1</v>
@@ -4353,13 +4362,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B65" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C65" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -4379,13 +4388,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B66" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C66" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
@@ -4405,13 +4414,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B67" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C67" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
@@ -4434,13 +4443,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B68" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C68" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -4460,13 +4469,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B69" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C69" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
@@ -4481,7 +4490,7 @@
         <v>4</v>
       </c>
       <c r="H69" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -4489,13 +4498,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B70" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C70" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D70" t="s">
         <v>13</v>
@@ -4515,13 +4524,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B71" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C71" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -4541,13 +4550,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B72" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C72" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -4567,13 +4576,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B73" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C73" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -4596,13 +4605,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B74" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C74" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -4617,7 +4626,7 @@
         <v>15</v>
       </c>
       <c r="H74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I74">
         <v>1</v>
@@ -4628,13 +4637,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B75" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -4649,7 +4658,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -4657,13 +4666,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B76" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C76" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -4686,13 +4695,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B77" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C77" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -4712,13 +4721,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B78" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C78" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -4738,13 +4747,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B79" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C79" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D79" t="s">
         <v>13</v>
@@ -4756,10 +4765,10 @@
         <v>15</v>
       </c>
       <c r="G79">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H79" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -4767,13 +4776,13 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B80" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C80" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D80" t="s">
         <v>13</v>
@@ -4785,10 +4794,10 @@
         <v>15</v>
       </c>
       <c r="G80">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H80" t="s">
-        <v>81</v>
+        <v>264</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -4796,13 +4805,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B81" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C81" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D81" t="s">
         <v>13</v>
@@ -4825,13 +4834,13 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B82" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C82" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D82" t="s">
         <v>13</v>
@@ -4846,7 +4855,7 @@
         <v>9</v>
       </c>
       <c r="H82" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="I82">
         <v>1</v>
@@ -4857,13 +4866,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B83" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C83" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D83" t="s">
         <v>13</v>
@@ -4883,13 +4892,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B84" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C84" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D84" t="s">
         <v>13</v>
@@ -4912,13 +4921,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B85" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C85" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D85" t="s">
         <v>13</v>
@@ -4938,13 +4947,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B86" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C86" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D86" t="s">
         <v>13</v>
@@ -4964,13 +4973,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B87" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C87" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D87" t="s">
         <v>13</v>
@@ -4990,13 +4999,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B88" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C88" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D88" t="s">
         <v>13</v>
@@ -5016,13 +5025,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B89" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C89" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D89" t="s">
         <v>13</v>
@@ -5042,13 +5051,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B90" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C90" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D90" t="s">
         <v>13</v>
@@ -5071,13 +5080,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B91" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C91" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D91" t="s">
         <v>13</v>
@@ -5092,7 +5101,7 @@
         <v>14</v>
       </c>
       <c r="H91" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="I91">
         <v>1</v>
@@ -5103,13 +5112,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B92" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C92" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D92" t="s">
         <v>13</v>
@@ -5129,13 +5138,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B93" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C93" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D93" t="s">
         <v>13</v>
@@ -5161,13 +5170,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B94" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C94" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D94" t="s">
         <v>13</v>
@@ -5187,13 +5196,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B95" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C95" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D95" t="s">
         <v>13</v>
@@ -5213,13 +5222,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B96" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C96" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D96" t="s">
         <v>13</v>
@@ -5245,13 +5254,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B97" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C97" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D97" t="s">
         <v>13</v>
@@ -5271,13 +5280,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B98" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C98" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D98" t="s">
         <v>13</v>
@@ -5292,7 +5301,7 @@
         <v>7</v>
       </c>
       <c r="H98" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="I98">
         <v>1</v>
@@ -5303,13 +5312,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B99" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C99" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D99" t="s">
         <v>13</v>
@@ -5329,13 +5338,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B100" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C100" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D100" t="s">
         <v>13</v>
@@ -5355,13 +5364,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B101" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C101" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D101" t="s">
         <v>13</v>
@@ -5381,13 +5390,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B102" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C102" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D102" t="s">
         <v>13</v>
@@ -5407,13 +5416,13 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B103" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C103" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D103" t="s">
         <v>13</v>
@@ -5433,13 +5442,13 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B104" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C104" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D104" t="s">
         <v>13</v>
@@ -5459,13 +5468,13 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B105" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C105" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D105" t="s">
         <v>13</v>
@@ -5485,13 +5494,13 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B106" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C106" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="D106" t="s">
         <v>13</v>
@@ -5506,7 +5515,7 @@
         <v>3</v>
       </c>
       <c r="H106" t="s">
-        <v>343</v>
+        <v>101</v>
       </c>
       <c r="I106">
         <v>0</v>
@@ -5514,13 +5523,13 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B107" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C107" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D107" t="s">
         <v>13</v>
@@ -5540,13 +5549,13 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B108" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C108" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D108" t="s">
         <v>13</v>
@@ -5566,13 +5575,13 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B109" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C109" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D109" t="s">
         <v>13</v>
@@ -5592,13 +5601,13 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B110" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C110" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D110" t="s">
         <v>13</v>
@@ -5618,13 +5627,13 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B111" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C111" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D111" t="s">
         <v>13</v>
@@ -5644,13 +5653,13 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B112" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C112" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D112" t="s">
         <v>13</v>
@@ -5670,13 +5679,13 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B113" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C113" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D113" t="s">
         <v>13</v>
@@ -5696,13 +5705,13 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B114" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C114" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D114" t="s">
         <v>13</v>
@@ -5725,13 +5734,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B115" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C115" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D115" t="s">
         <v>13</v>
@@ -5751,13 +5760,13 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B116" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C116" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D116" t="s">
         <v>13</v>
@@ -5777,13 +5786,13 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B117" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C117" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D117" t="s">
         <v>13</v>
@@ -5803,13 +5812,13 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B118" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C118" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D118" t="s">
         <v>13</v>
@@ -5829,13 +5838,13 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B119" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C119" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D119" t="s">
         <v>13</v>
@@ -5855,13 +5864,13 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B120" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C120" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D120" t="s">
         <v>13</v>
@@ -5881,13 +5890,13 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B121" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C121" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D121" t="s">
         <v>13</v>
@@ -5907,13 +5916,13 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B122" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C122" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D122" t="s">
         <v>13</v>
@@ -5933,13 +5942,13 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B123" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C123" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D123" t="s">
         <v>13</v>
@@ -5959,13 +5968,13 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B124" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C124" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D124" t="s">
         <v>13</v>
@@ -5985,13 +5994,13 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B125" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C125" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D125" t="s">
         <v>13</v>
@@ -6006,7 +6015,7 @@
         <v>3</v>
       </c>
       <c r="H125" t="s">
-        <v>343</v>
+        <v>101</v>
       </c>
       <c r="I125">
         <v>1</v>
@@ -6017,13 +6026,13 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B126" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C126" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D126" t="s">
         <v>13</v>
@@ -6049,13 +6058,13 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B127" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C127" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D127" t="s">
         <v>13</v>
@@ -6075,13 +6084,13 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B128" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C128" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D128" t="s">
         <v>13</v>
@@ -6104,13 +6113,13 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B129" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C129" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D129" t="s">
         <v>13</v>
@@ -6133,13 +6142,13 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B130" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C130" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D130" t="s">
         <v>13</v>
@@ -6154,7 +6163,7 @@
         <v>12</v>
       </c>
       <c r="H130" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="I130">
         <v>1</v>
@@ -6165,13 +6174,13 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B131" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C131" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D131" t="s">
         <v>13</v>
@@ -6191,13 +6200,13 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B132" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C132" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D132" t="s">
         <v>13</v>
@@ -6217,13 +6226,13 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B133" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C133" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D133" t="s">
         <v>35</v>
@@ -6243,13 +6252,13 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B134" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C134" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D134" t="s">
         <v>13</v>
@@ -6275,13 +6284,13 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B135" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C135" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D135" t="s">
         <v>13</v>
@@ -6301,13 +6310,13 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B136" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C136" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D136" t="s">
         <v>35</v>
@@ -6327,13 +6336,13 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B137" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C137" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D137" t="s">
         <v>13</v>
@@ -6353,13 +6362,13 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B138" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C138" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D138" t="s">
         <v>13</v>
@@ -6379,13 +6388,13 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B139" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C139" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D139" t="s">
         <v>13</v>
@@ -6405,13 +6414,13 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B140" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C140" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D140" t="s">
         <v>13</v>
@@ -6437,10 +6446,10 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C141" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D141" t="s">
         <v>13</v>
@@ -6455,7 +6464,7 @@
         <v>4</v>
       </c>
       <c r="H141" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="I141">
         <v>1</v>
@@ -6466,13 +6475,13 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B142" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C142" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D142" t="s">
         <v>13</v>
@@ -6492,13 +6501,13 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B143" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C143" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D143" t="s">
         <v>13</v>
@@ -6518,13 +6527,13 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B144" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C144" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D144" t="s">
         <v>13</v>
@@ -6544,13 +6553,13 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B145" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C145" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D145" t="s">
         <v>13</v>
@@ -6576,13 +6585,13 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B146" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C146" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D146" t="s">
         <v>13</v>
@@ -6602,13 +6611,13 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B147" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C147" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D147" t="s">
         <v>13</v>
@@ -6628,13 +6637,13 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B148" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C148" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D148" t="s">
         <v>13</v>
@@ -6654,13 +6663,13 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B149" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C149" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D149" t="s">
         <v>13</v>
@@ -6680,13 +6689,13 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B150" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C150" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D150" t="s">
         <v>13</v>
@@ -6706,13 +6715,13 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B151" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C151" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D151" t="s">
         <v>13</v>
@@ -6735,13 +6744,13 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B152" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C152" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D152" t="s">
         <v>13</v>
@@ -6753,10 +6762,10 @@
         <v>15</v>
       </c>
       <c r="G152">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H152" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="I152">
         <v>1</v>
@@ -6767,13 +6776,13 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B153" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C153" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D153" t="s">
         <v>13</v>
@@ -6782,13 +6791,13 @@
         <v>14</v>
       </c>
       <c r="F153" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G153">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H153" t="s">
-        <v>484</v>
+        <v>121</v>
       </c>
       <c r="I153">
         <v>1</v>
@@ -6799,13 +6808,13 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B154" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C154" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D154" t="s">
         <v>13</v>
@@ -6828,13 +6837,13 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B155" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C155" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D155" t="s">
         <v>13</v>
@@ -6854,13 +6863,13 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B156" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C156" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D156" t="s">
         <v>35</v>
@@ -6880,13 +6889,13 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B157" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C157" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D157" t="s">
         <v>13</v>
@@ -6909,13 +6918,13 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B158" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C158" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D158" t="s">
         <v>13</v>
@@ -6935,13 +6944,13 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B159" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C159" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D159" t="s">
         <v>35</v>
@@ -6961,13 +6970,13 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B160" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C160" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D160" t="s">
         <v>13</v>
@@ -6982,7 +6991,7 @@
         <v>3</v>
       </c>
       <c r="H160" t="s">
-        <v>343</v>
+        <v>101</v>
       </c>
       <c r="I160">
         <v>1</v>
@@ -6993,13 +7002,13 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B161" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C161" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D161" t="s">
         <v>13</v>
@@ -7019,13 +7028,13 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B162" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C162" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D162" t="s">
         <v>13</v>
@@ -7045,13 +7054,13 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B163" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C163" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D163" t="s">
         <v>13</v>
@@ -7071,13 +7080,13 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B164" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C164" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D164" t="s">
         <v>13</v>
@@ -7097,13 +7106,13 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B165" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C165" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D165" t="s">
         <v>13</v>
@@ -7123,13 +7132,13 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B166" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C166" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D166" t="s">
         <v>13</v>
@@ -7149,13 +7158,13 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B167" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C167" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D167" t="s">
         <v>13</v>
@@ -7175,13 +7184,13 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B168" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C168" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D168" t="s">
         <v>13</v>
@@ -7201,13 +7210,13 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B169" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C169" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D169" t="s">
         <v>13</v>
@@ -7227,13 +7236,13 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B170" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C170" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D170" t="s">
         <v>13</v>
@@ -7253,13 +7262,13 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B171" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C171" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D171" t="s">
         <v>13</v>
@@ -7279,13 +7288,13 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B172" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C172" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D172" t="s">
         <v>13</v>
@@ -7305,13 +7314,13 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B173" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C173" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D173" t="s">
         <v>13</v>
@@ -7326,7 +7335,7 @@
         <v>12</v>
       </c>
       <c r="H173" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="I173">
         <v>1</v>
@@ -7337,13 +7346,13 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B174" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C174" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D174" t="s">
         <v>13</v>
@@ -7363,13 +7372,13 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B175" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C175" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D175" t="s">
         <v>13</v>
@@ -7389,13 +7398,13 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B176" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C176" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D176" t="s">
         <v>13</v>
@@ -7415,13 +7424,13 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B177" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C177" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D177" t="s">
         <v>13</v>
@@ -7441,13 +7450,13 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B178" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C178" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D178" t="s">
         <v>13</v>
@@ -7467,13 +7476,13 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B179" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C179" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D179" t="s">
         <v>35</v>
@@ -7493,13 +7502,13 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B180" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C180" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D180" t="s">
         <v>35</v>
@@ -7519,13 +7528,13 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B181" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C181" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D181" t="s">
         <v>13</v>
@@ -7551,13 +7560,13 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B182" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C182" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D182" t="s">
         <v>13</v>

</xml_diff>